<commit_message>
finished custom name parser
</commit_message>
<xml_diff>
--- a/custom/logs/custom.xlsx
+++ b/custom/logs/custom.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13492" uniqueCount="6171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13493" uniqueCount="6172">
   <si>
     <t>FLOUR TORTILLA</t>
   </si>
@@ -18543,6 +18543,9 @@
   </si>
   <si>
     <t>Custom2</t>
+  </si>
+  <si>
+    <t>ITEM</t>
   </si>
 </sst>
 </file>
@@ -18861,9 +18864,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7918"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -18873,6 +18874,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>6171</v>
+      </c>
       <c r="B1" t="s">
         <v>6169</v>
       </c>

</xml_diff>